<commit_message>
Added Constituency Supervisor Menu
</commit_message>
<xml_diff>
--- a/Menu/staff.xlsx
+++ b/Menu/staff.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="7830" windowHeight="4845"/>
@@ -15,7 +15,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Staff!$A$1:$I$1</definedName>
     <definedName name="staffExported" localSheetId="0">Staff!$A$2:$I$54</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="257">
   <si>
     <t>Name</t>
   </si>
@@ -805,6 +805,12 @@
   </si>
   <si>
     <t>74</t>
+  </si>
+  <si>
+    <t>Maama Letsie</t>
+  </si>
+  <si>
+    <t>0099</t>
   </si>
 </sst>
 </file>
@@ -1153,12 +1159,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23:B23"/>
+      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2556,6 +2562,17 @@
       <c r="F54" s="4"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B55" t="s">
+        <v>255</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:I54">

</xml_diff>

<commit_message>
Everyone who appears on the household roaster can be a proxy. If a person says his/main activity is Student, then s/he must be attending and not the other way round
</commit_message>
<xml_diff>
--- a/Menu/staff.xlsx
+++ b/Menu/staff.xlsx
@@ -861,9 +861,9 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1085,8 +1085,8 @@
         <v>1</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f>CONCATENATE(E9,F9,RIGHT(G9,2),H9,I9,"0",J9)</f>
-        <v>043611110</v>
+        <f>CONCATENATE(E9,F9,RIGHT(G9,2),H9,I9,"0",J9,"98")</f>
+        <v>04361111098</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>18</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2" t="str">
-        <f>CONCATENATE(B16,C16,RIGHT(D16,2),E16,F16,"0",G16)</f>
+        <f t="shared" ref="A16:A21" si="0">CONCATENATE(B16,C16,RIGHT(D16,2),E16,F16,"0",G16)</f>
         <v>02131211050</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1793,7 +1793,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2" t="str">
-        <f>CONCATENATE(B17,C17,RIGHT(D17,2),E17,F17,"0",G17)</f>
+        <f t="shared" si="0"/>
         <v>02131211058</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1817,7 +1817,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2" t="str">
-        <f>CONCATENATE(B18,C18,RIGHT(D18,2),E18,F18,"0",G18)</f>
+        <f t="shared" si="0"/>
         <v>02131211067</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1841,7 +1841,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2" t="str">
-        <f>CONCATENATE(B19,C19,RIGHT(D19,2),E19,F19,"0",G19)</f>
+        <f t="shared" si="0"/>
         <v>02131211074</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1865,7 +1865,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2" t="str">
-        <f>CONCATENATE(B20,C20,RIGHT(D20,2),E20,F20,"0",G20)</f>
+        <f t="shared" si="0"/>
         <v>02131211084</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1889,7 +1889,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="2" t="str">
-        <f>CONCATENATE(B21,C21,RIGHT(D21,2),E21,F21,"0",G21)</f>
+        <f t="shared" si="0"/>
         <v>02131211097</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2057,7 +2057,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2" t="str">
-        <f>CONCATENATE(B28,C28,RIGHT(D28,2),E28,F28,G28)</f>
+        <f t="shared" ref="A28:A34" si="1">CONCATENATE(B28,C28,RIGHT(D28,2),E28,F28,G28)</f>
         <v>02140812115</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2081,7 +2081,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="2" t="str">
-        <f>CONCATENATE(B29,C29,RIGHT(D29,2),E29,F29,G29)</f>
+        <f t="shared" si="1"/>
         <v>02141211140</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2105,7 +2105,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="2" t="str">
-        <f>CONCATENATE(B30,C30,RIGHT(D30,2),E30,F30,G30)</f>
+        <f t="shared" si="1"/>
         <v>02141211184</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2129,7 +2129,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2" t="str">
-        <f>CONCATENATE(B31,C31,RIGHT(D31,2),E31,F31,G31)</f>
+        <f t="shared" si="1"/>
         <v>02151311128</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2153,7 +2153,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="2" t="str">
-        <f>CONCATENATE(B32,C32,RIGHT(D32,2),E32,F32,G32)</f>
+        <f t="shared" si="1"/>
         <v>02151311145</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2177,7 +2177,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="2" t="str">
-        <f>CONCATENATE(B33,C33,RIGHT(D33,2),E33,F33,G33)</f>
+        <f t="shared" si="1"/>
         <v>02160912137</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -2201,7 +2201,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="2" t="str">
-        <f>CONCATENATE(B34,C34,RIGHT(D34,2),E34,F34,G34)</f>
+        <f t="shared" si="1"/>
         <v>02160912181</v>
       </c>
       <c r="B34" s="1" t="s">

</xml_diff>

<commit_message>
Added a function to display household summary report by date.
</commit_message>
<xml_diff>
--- a/Menu/staff.xlsx
+++ b/Menu/staff.xlsx
@@ -815,10 +815,17 @@
     <numFmt numFmtId="164" formatCode="0000"/>
     <numFmt numFmtId="165" formatCode="00"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -844,12 +851,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1156,9 +1167,9 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23:B23"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1289,32 +1300,32 @@
         <v>238</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:9" s="6" customFormat="1">
+      <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="8" t="s">
         <v>238</v>
       </c>
     </row>
@@ -1753,32 +1764,32 @@
         <v>238</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:9" s="6" customFormat="1">
+      <c r="A21" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="C21" s="6">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="8" t="s">
         <v>238</v>
       </c>
     </row>
@@ -1840,32 +1851,32 @@
         <v>238</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:9" s="6" customFormat="1">
+      <c r="A24" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C24" s="6">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="8" t="s">
         <v>238</v>
       </c>
     </row>
@@ -2188,32 +2199,32 @@
         <v>238</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:9" s="6" customFormat="1">
+      <c r="A36" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36" s="2" t="s">
+      <c r="C36" s="6">
+        <v>1</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="H36" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="I36" s="3" t="s">
+      <c r="H36" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="I36" s="8" t="s">
         <v>239</v>
       </c>
     </row>

</xml_diff>